<commit_message>
changes in Excel file and fix reading issue by adding DataFormatter class
</commit_message>
<xml_diff>
--- a/TestData/UserData.xlsx
+++ b/TestData/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/eclipse-workspace/Framework/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D343FC-DB39-F542-A98E-F59E500FA992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55852C02-88B5-284A-9EF3-2D2DA4150EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{AA21495F-C6C0-594B-9612-85490FAA987A}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{AA21495F-C6C0-594B-9612-85490FAA987A}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,10 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>osama@mavrictech.com</t>
+    <t>Chrome</t>
   </si>
   <si>
-    <t>Chrome</t>
+    <t>osama@mavrictech.com</t>
   </si>
 </sst>
 </file>
@@ -92,9 +92,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -413,39 +414,42 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>12345678</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3380BB3E-8560-BB44-A812-6D8DE6E71AC0}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE63C0B1-37D9-CC4B-A6EC-1B461DBD6012}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>